<commit_message>
added who is God
</commit_message>
<xml_diff>
--- a/Jehovah Witness.xlsx
+++ b/Jehovah Witness.xlsx
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added clean you can be God's Friend
</commit_message>
<xml_diff>
--- a/Jehovah Witness.xlsx
+++ b/Jehovah Witness.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="275">
   <si>
     <t>Adhola</t>
   </si>
@@ -835,12 +835,33 @@
   <si>
     <t>Machien</t>
   </si>
+  <si>
+    <t>Were Mito Ni Ibedi Mere Pere</t>
+  </si>
+  <si>
+    <t>Go lakonyin limo kisangala i kwo.</t>
+  </si>
+  <si>
+    <t>Ginaŋo manyalo konyin ŋeyo gima go mito kodi gima go kimiti.</t>
+  </si>
+  <si>
+    <t>Go konyo wan ŋeyo gima go otimo cango con, gima go tima pama, kodi gima go latimo i hongo mabino.</t>
+  </si>
+  <si>
+    <t>Piny manyien k’obedi paka piny ma wan’iye pama. Piny manyien ochale nedi?</t>
+  </si>
+  <si>
+    <t>Aŋo manyutho?</t>
+  </si>
+  <si>
+    <t>Gima Baibul waco ri wan kwoŋ mikula ma ndir pa Nowa fonjo wan aŋo?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,6 +910,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -920,7 +947,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -939,6 +966,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1234,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2007,8 +2035,44 @@
         <v>256</v>
       </c>
     </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="15.75">
+      <c r="A99" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="30">
+      <c r="A100" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="30">
+      <c r="A101" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="30">
+      <c r="A103" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2017,7 +2081,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added Listen to God and Live
</commit_message>
<xml_diff>
--- a/Jehovah Witness.xlsx
+++ b/Jehovah Witness.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="1" r:id="rId1"/>
     <sheet name="Common Verbs" sheetId="3" r:id="rId2"/>
+    <sheet name="Listen to God" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="736">
   <si>
     <t>Adhola</t>
   </si>
@@ -884,12 +885,1379 @@
   <si>
     <t>Piny manyien ochale nedi?</t>
   </si>
+  <si>
+    <t>Ji jowinjo wach pa Were kis Kamoro</t>
+  </si>
+  <si>
+    <t>People everywhere are listening.</t>
+  </si>
+  <si>
+    <t>Jehova omiyo Adam kodi Eva gikipiny mabeyo kweth</t>
+  </si>
+  <si>
+    <t>Jehovah created everything in heaven . . . and on earth.</t>
+  </si>
+  <si>
+    <t>Jehova ochweyo gikipiny jye manitye ipolo kodi i piny</t>
+  </si>
+  <si>
+    <t>Jehovah gave Adam and Eve many good things.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were ochiero jo chamo kwo  yath achiel. </t>
+  </si>
+  <si>
+    <t>God said not to eat from one of the trees.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam kodi Eva jokowinjo Were, amomiyo jotho. </t>
+  </si>
+  <si>
+    <t>Adam and Eve did not obey God, so they died.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paka fukefuke ongoye gi kwo, jomotho bende jongoye gi kwo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joma thoth indir pa Nowa jotimo gikipiny marecho. </t>
+  </si>
+  <si>
+    <t>The dead are as lifeless as the dust.</t>
+  </si>
+  <si>
+    <t>Most in Noah’s time did what was bad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowa owinjo Were to geto yee. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were oreyo woko jomarecho tobotho Nowa kodi jopecho pere. </t>
+  </si>
+  <si>
+    <t>Noah listened to God and built an ark.</t>
+  </si>
+  <si>
+    <t>God destroyed the wicked but saved Noah and his family.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odoko Were chiegin reyo woko jomarecho to botho joma beyo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jehova ooro Yesu ipiny. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kada nende Yesu otimo gikipiny mabeyo, komar go. </t>
+  </si>
+  <si>
+    <t>God will again destroy the wicked and save the good people.</t>
+  </si>
+  <si>
+    <t>Jehovah sent Jesus to earth.</t>
+  </si>
+  <si>
+    <t>Jesus did good but was hated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yesu otho_x0002_ney wanyal limokwo. </t>
+  </si>
+  <si>
+    <t>Were ochierino Yesu to loko go Kere ma Ker pa Were</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chandirok manitye ipiny nyutho ni Ker pa Were chiegin bino. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ker pa Were bino kwanyo woko gikipiny marecho jye. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jomotho jobino chierino jobedi ipinyka. </t>
+  </si>
+  <si>
+    <t>Jesus died so that we might live.</t>
+  </si>
+  <si>
+    <t>God resurrected Jesus and made him King of God’s Kingdom.</t>
+  </si>
+  <si>
+    <t>Troubles on the earth prove that God’s Kingdom will soon act.</t>
+  </si>
+  <si>
+    <t>The Kingdom will remove all wickedness.</t>
+  </si>
+  <si>
+    <t>Most of the dead will be resurrected on earth.</t>
+  </si>
+  <si>
+    <t>God’s Kingdom will end all suffering.</t>
+  </si>
+  <si>
+    <t>God does hear our prayers.</t>
+  </si>
+  <si>
+    <t>We can pray about many things.</t>
+  </si>
+  <si>
+    <t>Ker pa Were bino kwanyo woko chandirok jye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were winjo kwayo mawan. </t>
+  </si>
+  <si>
+    <t>Wanyalo kwayo kwo_x0002_ gimoro jye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar amakelo kisangala ipecho. </t>
+  </si>
+  <si>
+    <t>Bedi dhano ma woro ji kendo magenere, ma kiweno dhano mager makigenere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ikiri itimi gimarach. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timi gimaber. </t>
+  </si>
+  <si>
+    <t>Bedi yuthenge pa Were.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Or ryeko munyo iyero giratima—winji Were. </t>
+  </si>
+  <si>
+    <t>Love is the key to happy families.</t>
+  </si>
+  <si>
+    <t>Be kind and faithful, not cruel and unfaithful.</t>
+  </si>
+  <si>
+    <t>Avoid what is bad.</t>
+  </si>
+  <si>
+    <t>Do what is good.</t>
+  </si>
+  <si>
+    <t>Take your stand on God’s side.</t>
+  </si>
+  <si>
+    <t>Make the right choice​—listen to God.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were chale gi janywolma maro nyithindho pere. </t>
+  </si>
+  <si>
+    <t>Baibul wacho ni: ‘Joma jowinjan, Amiyo jo kwo makirum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were oro Baibul luwo kodi wan. </t>
+  </si>
+  <si>
+    <t>God is like a loving father.</t>
+  </si>
+  <si>
+    <t>God speaks to us through the Bible.</t>
+  </si>
+  <si>
+    <t>The Bible says: 'Those who listen to me, I give them everlasting life'</t>
+  </si>
+  <si>
+    <t>Winji Were</t>
+  </si>
+  <si>
+    <t>Listen to God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">God is our Creator, and he cares for us. </t>
+  </si>
+  <si>
+    <t>God reveals precious truths that fill us with joy and hope.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+If you listen to God, he will guide and protect you and help you deal with problems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+But there is more​—you will live forever!</t>
+  </si>
+  <si>
+    <t>Kareno nitye kir gima loyo meno
+—ibino limo kwo makirum!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just as a wise and loving father instructs his children, </t>
+  </si>
+  <si>
+    <t>Likewise, God teaches people everywhere the best way to live.</t>
+  </si>
+  <si>
+    <t>Janywol maryek kendo mani gi mar,
+fuonjo nyithindho pere.</t>
+  </si>
+  <si>
+    <t>Ka iwinjo Were, go bino miyin ryeko kendo bino konyin i teko moro jye.</t>
+  </si>
+  <si>
+    <t>Ameno apaka Were bende fuonjo ji pere
+nger malimo kwo maber.</t>
+  </si>
+  <si>
+    <t>Were fuonjo wan adyeri ma kelo ri wan kisangala kendo ma miyo
+wan geno.</t>
+  </si>
+  <si>
+    <t>Were amochweyo wan, aka go dewo kwo wan swa</t>
+  </si>
+  <si>
+    <t>Were Luwo Kodi Wan Nedi?</t>
+  </si>
+  <si>
+    <t>Were mito ni kis dhano manitye i piny osoma Baibul Baibul nwaere i dhudhok makweth.</t>
+  </si>
+  <si>
+    <t>Ka imito winjo Were, iripo kisoma kendo inia gima Baibul wacho.</t>
+  </si>
+  <si>
+    <t>If you want to listen to God, you must read and understand the Bible.</t>
+  </si>
+  <si>
+    <t>Chango chon, Were maradyeri ooro ji ndiko paro pere i kitawo achiel male milwoo ni Baibul</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kitawo no n’iye wach maber ma Were mito ni ieyi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ka inowinji go ibino bedo dhano maryek.</t>
+  </si>
+  <si>
+    <t>Were oeyo gimaber ri wan aka ryeko jye wok bonge.</t>
+  </si>
+  <si>
+    <t>The true God directed men to write down his thoughts in one sacred book called the Bible</t>
+  </si>
+  <si>
+    <t>It contains important information that God wants you to know.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> By listening to him, you will become truly wise.​</t>
+  </si>
+  <si>
+    <t>God knows what is best for us, and he is the Source of all wisdom.</t>
+  </si>
+  <si>
+    <t>God wants everyone on earth to read the Bible which is now available in many languages.</t>
+  </si>
+  <si>
+    <t>How Does God speak to us?</t>
+  </si>
+  <si>
+    <t>Wajulizi pa Jehova jonyalo konyin fuonjirok Baibul.</t>
+  </si>
+  <si>
+    <t>I piny gipi, jofuonjo adyeri ma mako kwo Were.</t>
+  </si>
+  <si>
+    <t>Jehovah’s Witnesses can help you understand the Bible.</t>
+  </si>
+  <si>
+    <t>In all the earth, they teach the truth about God.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ikiripere chulo pesa moro jye nyalo limo fuonji me. </t>
+  </si>
+  <si>
+    <t>You do not have to pay anything for this instruction. Y</t>
+  </si>
+  <si>
+    <t>Ka chokirok no ilwoo ni Kingdom Hall of Jehovah’s Witnesses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inyalo kir fuonjere kwo Were ka ikidho ka chokirok pa Wajulizi pa Jehova. </t>
+  </si>
+  <si>
+    <t>Those meeting places are called  Kingdom Hall of Jehovah’s Witnesses.</t>
+  </si>
+  <si>
+    <t>You can also learn about God when you attend  Jehovah Witness meetings</t>
+  </si>
+  <si>
+    <t>Wach pa Were obedo adyeri.</t>
+  </si>
+  <si>
+    <t>Irao wanyalo geno Were?</t>
+  </si>
+  <si>
+    <t>Why can we trust in God?​</t>
+  </si>
+  <si>
+    <t>God’s word is truth.​</t>
+  </si>
+  <si>
+    <t>Were Maradyeri a a?</t>
+  </si>
+  <si>
+    <t>Who Is the True God?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitye Were achiel kende maradyeri, aka ilwoo go ni Jehova. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is only one true God, and his name is Jehovah. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> He also wants us to love other people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> He is the Supreme One, the Creator of all things.</t>
+  </si>
+  <si>
+    <t>Go obedo chuny, wakinyal neno go.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Go maro wan aka go mito ni wabende wamar go. </t>
+  </si>
+  <si>
+    <t>Kendo go mito ni wamar jowoti wan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Go a Were Majameni jye, Jachwech ma gikipiny jye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He is a Spirit; we cannot see him. </t>
+  </si>
+  <si>
+    <t>He loves us and wants us to love him in return.</t>
+  </si>
+  <si>
+    <t>Jehova amochweyo kir jomalaika.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo obino i piny olwo
+go ni Yesu Kristo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first of God’s creations was a mighty spirit person </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Later he came to earth ans was called  Jesus Christ</t>
+  </si>
+  <si>
+    <t>Chwech pa Were marapena obedo dhano ma chuny majameni.</t>
+  </si>
+  <si>
+    <t>Jehovah also created the angels.</t>
+  </si>
+  <si>
+    <t>Jehova ochweyo michalin, piny kodi gikipiny jye man’iy</t>
+  </si>
+  <si>
+    <t>Jehovah God created the stars as well as the earth and all that is on it</t>
+  </si>
+  <si>
+    <t>He formed Adam, the first man, from the dust of the ground.​</t>
+  </si>
+  <si>
+    <t>Why should we honor Jehovah?​</t>
+  </si>
+  <si>
+    <t>What are some of God’s qualities?​</t>
+  </si>
+  <si>
+    <t>Ochweyo Adam, dhano marapena, wok i fukefuke.</t>
+  </si>
+  <si>
+    <t>Irao waripo miyo Jehova wor?</t>
+  </si>
+  <si>
+    <t>Megi kwo kite pa Were a mene?</t>
+  </si>
+  <si>
+    <t>Kwo Oido Chale Nedi i Ndelo ma Eden?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jehova ochweyo dhako motelo milwoo ni Eva, to miyo Adam dhako no wobedi chiege. </t>
+  </si>
+  <si>
+    <t>Jehova ochweyo jo munyo joni gi paro kanyachiel gi kwo maber, jokobedo gi teko moro jye.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pecho pajo maon oido ilwoo ni ndelo ma Eden —jwom, yen manyak girachama kodi ogwange jye oido nitye kanyago.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jehova oido luwo gi jo kanyachiel gi fuonjo jo; bedi jowinjo go di jobedo i piny ka chil gi chil.</t>
+  </si>
+  <si>
+    <t>What Was Life Like in Paradise?</t>
+  </si>
+  <si>
+    <t>Jehovah created them with minds and bodies that were perfect, without any flaw.</t>
+  </si>
+  <si>
+    <t>Jehovah made the first woman, Eve, and gave her to Adam to be his wife</t>
+  </si>
+  <si>
+    <t>Their Paradise home was the garden of Eden​—a place of great beauty with a river and fruit trees and animals.</t>
+  </si>
+  <si>
+    <t>Jehovah spoke to them; he taught them. If they listened to him, they would live forever in Paradise on earth.</t>
+  </si>
+  <si>
+    <t>Jehovah showed Adam and Eve one fruit tree in the garden and told them that if they ate from it, they would die.</t>
+  </si>
+  <si>
+    <t>Malaika achiel ochayo Were.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of the angels rebelled against God. </t>
+  </si>
+  <si>
+    <t>That wicked angel is Satan the Devil.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Malaika marach no ilwoo ni Sitan. </t>
+  </si>
+  <si>
+    <t>Jehova onyutho Adam kodi Eva yath achiel mobedo i ndelo ma Eden to wacho ri jo ni ka jochamo kwo yath no jobino tho.</t>
+  </si>
+  <si>
+    <t>Satan did not want Adam and Eve to obey Jehovah.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sitan komito ni Adam kodi Eva jowinji Jehova. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ri ameno munyo oro thwol, Sitan owacho ri Eva ni ka jochamo kwo yath no jokiletho, kwanyo woko jolebedo paka Were. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To meno obedo twodo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> So he used a serpent to tell Eve that if she ate the fruit from that tree, she would not die, but she would be like God. </t>
+  </si>
+  <si>
+    <t>Of course, that was a lie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eva owinjo thwol to chamo kwo yath ma Were ochiero jo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rumachien to miyo Adam bende to chamo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Were oryemo jo i ndelo ma Eden. </t>
+  </si>
+  <si>
+    <t>Kwo obedo ri jo matek kanyachiel gi nyithindho pajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Joti to jotho. </t>
+  </si>
+  <si>
+    <t>Ongoye kama jokidh’iye; kwo pajo orumo kichutho.</t>
+  </si>
+  <si>
+    <t>Ginao Mowok’iye?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jowinjo Sitan </t>
+  </si>
+  <si>
+    <t>With What Results?</t>
+  </si>
+  <si>
+    <t>They Listened to Satan​</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eve listened to the serpent and ate of the fruit. </t>
+  </si>
+  <si>
+    <t>Afterward, she gave some to Adam, and he ate it.</t>
+  </si>
+  <si>
+    <t>God made them leave their Paradise home.</t>
+  </si>
+  <si>
+    <t>What they did was wrong​</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it was a sin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gima jotimo kobedo gimotire </t>
+  </si>
+  <si>
+    <t>obedo gimarach.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life was hard for them and their children. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">They grew old and died. </t>
+  </si>
+  <si>
+    <t>They did not go to the spirit world; they ceased to exist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We die because we all come from Adam and Eve. </t>
+  </si>
+  <si>
+    <t>The dead are not able to see or hear or do anything.</t>
+  </si>
+  <si>
+    <t>Jehovah did not mean for people to die.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soon he will bring back to life those asleep in death.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If they listen to him, they will live forever.</t>
+  </si>
+  <si>
+    <t>Why do we die?​</t>
+  </si>
+  <si>
+    <t>Death will be no more.​</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watho rupiri wajojye wabedo nyikway
+Adam gi Eva. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jochale pa dhano ma nindo.</t>
+  </si>
+  <si>
+    <t>Jomotho jokinyal neno kosa winjo kosa timo gimoro jye.</t>
+  </si>
+  <si>
+    <t>They are like those who are asleep</t>
+  </si>
+  <si>
+    <t>Tho kobedo atoa pa Were ri ji.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jehova chiegin chierino jomotho. </t>
+  </si>
+  <si>
+    <t>Ka jowinji go, jobino limo kwo makirum.</t>
+  </si>
+  <si>
+    <t>Tho bino rumo woko kichutho.</t>
+  </si>
+  <si>
+    <t>Irao watho?</t>
+  </si>
+  <si>
+    <t>Mikula ma Ndir pa Nowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jomene ma Jowinjo Were? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam kodi Eva jonywolo nyithindho to ji jomedere i piny. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rumachien, jomalaika megi jomakere gi Sitan to jochayo Were. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jobino i piny to jolokere ji to jonywomo mon. </t>
+  </si>
+  <si>
+    <t>Nyithindho ma mon no jonywolo oido jombo loyo dhano moro jye, oido joger aka oido joni gi men moasere.</t>
+  </si>
+  <si>
+    <t>Who Listened to God</t>
+  </si>
+  <si>
+    <t>The Great Flood​ during Noah's time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They came to earth and took on the bodies of men so that they could marry women. </t>
+  </si>
+  <si>
+    <t>The women gave birth to superhuman sons, who were fierce and strong.</t>
+  </si>
+  <si>
+    <t>Adam and Eve had children, and people became many on the earth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In time, some angels joined Satan’s rebellion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The world became filled with people who did bad things. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Piny obino opo’iye ji marecho.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> man’s wickedness was great on the earth and that every inclination of the thoughts of his heart was only bad all the time.</t>
+  </si>
+  <si>
+    <t>Recho pa dhano obino opo i piny gipi aka paro pere jye oido rach hongo jye.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noah was a good man. </t>
+  </si>
+  <si>
+    <t>Jehovah told Noah that He was going to destroy the wicked people with a great flood.</t>
+  </si>
+  <si>
+    <t>God also told Noah to build a huge boat, called an ark, and to take into it his family and every sort of animal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noah warned people about the coming Flood, but they did not listen. </t>
+  </si>
+  <si>
+    <t>Some laughed at Noah; others hated him.</t>
+  </si>
+  <si>
+    <t>When the ark was finished, Noah brought the animals inside.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowa obedo dhano maber. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jehova owacho ri Nowa nike kidho reyo woko ji jye gi mikula. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were owacho ri Nowa geto yee madwo swa, orwak’iye jopecho pere kodi ogwange mopokere opokere. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowa owacho ri ji kwo mikula moido kidho bino, to jokowinjo go. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jomegi jonyiero go; jomegi oido jomon gi go. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo geto yee orumo, Nowa orwak’iye ogwange. </t>
+  </si>
+  <si>
+    <t>Nowa kodi jopecho pere to bende jodonjo i yee</t>
+  </si>
+  <si>
+    <t>Noah and his family entered too.</t>
+  </si>
+  <si>
+    <t>What Do We Learn From the Great Flood?</t>
+  </si>
+  <si>
+    <t>The rebellious angels left their bodies of flesh and became demons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It rained for 40 days and 40 nights, and the water covered all the earth. </t>
+  </si>
+  <si>
+    <t>All the wicked people died.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Though Noah and his family eventually died, God will bring them to life again with the prospect of living forever.</t>
+  </si>
+  <si>
+    <t>Those who were in the ark survived.</t>
+  </si>
+  <si>
+    <t>Ginao ma Wafuonjere Kwo Mikula ma Ndir pa Nowa?</t>
+  </si>
+  <si>
+    <t>Koth ochwe ndelo 40, wor g’odyechie, to umo piny gipi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ji marecho jye jotho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Jomalaika marecho jolunyo del
+pajo to jolokere jwogi.</t>
+  </si>
+  <si>
+    <t>Joma jobedo i yee joboth.</t>
+  </si>
+  <si>
+    <t>Kada nende Nowa kodi jopecho pere jotho rumachien, jobino chierino jolimi kwo makirum.</t>
+  </si>
+  <si>
+    <t>Sitan kodi jwogi fuodi jomedere wondo ji.</t>
+  </si>
+  <si>
+    <t>Jomarecho ibino reyo woko jo aka joma mwol jobino bedo i piny.</t>
+  </si>
+  <si>
+    <t>Yeri royo ma tero jo i kwo.</t>
+  </si>
+  <si>
+    <t>Jowinjo Were to jotimo gima Were wacho; jono ilwoo jo ni Wajulizi pa Jehova.</t>
+  </si>
+  <si>
+    <t>Jomegi jochale gi Nowa.</t>
+  </si>
+  <si>
+    <t>Satan and the demons continue to mislead people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soon Jehovah will destroy all who are wicked.</t>
+  </si>
+  <si>
+    <t>Today, as in Noah’s time, many reject Jehovah’s loving direction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Konon, paka obedo I ndir pa Nowa, joma thoth jokiwinji Jehova.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jehova bino reyo woko jomarecho jye.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some people are like Noah. </t>
+  </si>
+  <si>
+    <t>They listen to God and do what he says; they are Jehovah’s Witnesses.</t>
+  </si>
+  <si>
+    <t>Choose the road that leads to life.​</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yesu Obedo a? </t>
+  </si>
+  <si>
+    <t>Ka wamito ni Jehova osangala, waripo winjo dhano man madwo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chango chon ma fuodi Jevova kochweyo Adam, Jehova ochweyo ato i polo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo hongo okadho, Jehova ooro go i piny ka.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dhako ma fuodi kuya jachwo milwoo ni Maria to nywolo go. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nyathi no ochwoki nyinge ni Yesu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo nitye i piny ka, Yesu onyutho kite pa Were. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ofuonjo ji adyeri ma mako kwo Were gi miseni.</t>
+  </si>
+  <si>
+    <t>Go obedo jawor, jamar, kendo dhano mayot tiyirok gine.</t>
+  </si>
+  <si>
+    <t>Who Was Jesus?</t>
+  </si>
+  <si>
+    <t>The wicked will be destroyed; the meek will stay on earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If we want to please Jehovah, we must listen to another important person. </t>
+  </si>
+  <si>
+    <t>Long before creating Adam, Jehovah created a mighty spirit person in the heavens.</t>
+  </si>
+  <si>
+    <t>The child was given the name Jesus.</t>
+  </si>
+  <si>
+    <t>A virgin named Mary gave birth to him</t>
+  </si>
+  <si>
+    <t>In time, Jehovah sent him to earth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a man on earth, Jesus perfectly reflected God’s qualities. </t>
+  </si>
+  <si>
+    <t>He was kind, loving, and approachable.</t>
+  </si>
+  <si>
+    <t>Fearlessly, he taught others the truth about Jehovah.</t>
+  </si>
+  <si>
+    <t>Jesus also healed the sick and raised to life some who had died.</t>
+  </si>
+  <si>
+    <t>The religious leaders hated Jesus because he exposed their false teachings and their evil ways.</t>
+  </si>
+  <si>
+    <t>The religious leaders persuaded the Romans to beat Jesus and to kill him.</t>
+  </si>
+  <si>
+    <t>What did Jesus do in heaven before he came to earth?​</t>
+  </si>
+  <si>
+    <t>Why is it important to know about Jesus?​</t>
+  </si>
+  <si>
+    <t>Yesu obotho jotwo to chierino kir jomotho.</t>
+  </si>
+  <si>
+    <t>Jotel ma din oido jodak Yesu rupiri Yesu otucho ri jo fuonji pajo matwodo kodi kula pajo marecho.</t>
+  </si>
+  <si>
+    <t>Jotel ma din joluwo twodo kwo Yesu momiyo Joroma jogoyo go to joneko.</t>
+  </si>
+  <si>
+    <t>Irao ber ni waey gima mako kwo Yesu?</t>
+  </si>
+  <si>
+    <t>Ginao ma Yesu otimo i polo munyo fuodi kobino i piny?</t>
+  </si>
+  <si>
+    <t>Tho pa Yesu Konyin Nedi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rumachien ma ndelo adek munyo Yesu otyeko tho, nitye mon ma jokidho kama oido oyik’iye go to jokonwao del pere. </t>
+  </si>
+  <si>
+    <t>Jehova oido otyeko chierino Yesu.</t>
+  </si>
+  <si>
+    <t>Rumachien, Yesu oneno ri jofuonjirok pere.</t>
+  </si>
+  <si>
+    <t>Jehova ochierino Yesu odoko Yesu to lokere chwech ma chuny makitho.</t>
+  </si>
+  <si>
+    <t>Jofuonjirok pa Yesu joneno go munyo gik i polo.</t>
+  </si>
+  <si>
+    <t>“Kemba” pa gimarach obedo ginao?</t>
+  </si>
+  <si>
+    <t>Yesu oyawo ri wan royo ma limo kwo makirum.</t>
+  </si>
+  <si>
+    <t>What Does the Death of Jesus Mean for You?</t>
+  </si>
+  <si>
+    <t>Three days after Jesus died, some women visited his tomb and found it empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jehovah had raised Jesus from the dead.</t>
+  </si>
+  <si>
+    <t>Jesus opened the way to everlasting life.</t>
+  </si>
+  <si>
+    <t>What are “the wages” of sin?​</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jesus’ disciples saw him go up to heaven.</t>
+  </si>
+  <si>
+    <t>Yes, Jehovah had resurrected Jesus to life as a powerful, immortal spirit creature.</t>
+  </si>
+  <si>
+    <t>Jesus later appeared to his apostles.</t>
+  </si>
+  <si>
+    <t>Yesu omiyo kwo pere paka chul ri ji jye.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luwo kwo chul no, Were bino miyo wan kwo makirum. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jehova oyero Yesu bedo Kere ma ledhumo piny. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ji 144,000 jolechierino wok i piny to jokidho i polo. </t>
+  </si>
+  <si>
+    <t>Yesu kodi ji 144,000 joledhum i Ker pa Were ma polo.</t>
+  </si>
+  <si>
+    <t>Ker pa Were bino loko piny me kabedo maber swa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lweny, turo chik, chandi, kodi kech jye bino rumo woko.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ji jolebedo i kisangala madit swa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Silwany mene ma Ker pa Were lekelo ri wan? </t>
+  </si>
+  <si>
+    <t>Waripo kwayo Ker pa Were wobin.</t>
+  </si>
+  <si>
+    <t>Jesus gave up his life to pay a ransom for mankind.</t>
+  </si>
+  <si>
+    <t>By means of that ransom, God makes it possible for us to live forever.</t>
+  </si>
+  <si>
+    <t>Jehovah appointed Jesus as King to rule over the earth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> With him will be 144,000 faithful people who are resurrected from the earth to life in heaven. </t>
+  </si>
+  <si>
+    <t>Jesus and the 144,000 form a righteous heavenly government​—God’s Kingdom.​</t>
+  </si>
+  <si>
+    <t xml:space="preserve">God’s Kingdom will make the earth a paradise. </t>
+  </si>
+  <si>
+    <t>War, crime, poverty, and hunger will be no more</t>
+  </si>
+  <si>
+    <t>People will be truly happy</t>
+  </si>
+  <si>
+    <t>What blessings will God’s Kingdom bring?​</t>
+  </si>
+  <si>
+    <t>We should pray for God’s Kingdom to come.​</t>
+  </si>
+  <si>
+    <t>When Will Paradise Come?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Bible foretold many of the things that are happening today. </t>
+  </si>
+  <si>
+    <t>There would be great earthquakes, wars, food shortages, and widespread disease</t>
+  </si>
+  <si>
+    <t>It said that people would be lovers of money, disobedient to parents, fierce, and lovers of pleasures.</t>
+  </si>
+  <si>
+    <t>These things are happening now.</t>
+  </si>
+  <si>
+    <t>Also, Jesus said that the good news about the Kingdom would be preached in all the earth.​</t>
+  </si>
+  <si>
+    <t>Jehovah will soon destroy all the wicked.</t>
+  </si>
+  <si>
+    <t>Satan and the demons will be punished.</t>
+  </si>
+  <si>
+    <t>Those who listen to God will survive into a righteous new world, where there will be no more fear, a world where people trust and love one another.</t>
+  </si>
+  <si>
+    <t>What did Jesus say would occur in our time?</t>
+  </si>
+  <si>
+    <t>The wicked will be destroyed.​</t>
+  </si>
+  <si>
+    <t>Piny pa Were Manyien Obin Kerao?</t>
+  </si>
+  <si>
+    <t>Baibul chango oluwo kwo gikipiny matimere pama.</t>
+  </si>
+  <si>
+    <t>Owacho ni ji di jobedo jomawor i pesa, joma kiwinji jonywol pajo, jomager, kodi joma maro kisangala ma piny.</t>
+  </si>
+  <si>
+    <t>Kendo Yesu owacho ni wach maber ma mako kwo Ker pa Were ibino fuonjo I piny gipi.</t>
+  </si>
+  <si>
+    <t>Yengirok ma piny, lweny, kech, kodi two ma kiboth.</t>
+  </si>
+  <si>
+    <t>Gikipiny me jye nitye konon.</t>
+  </si>
+  <si>
+    <t>Jehova chiegin reyo woko jomarecho jye.</t>
+  </si>
+  <si>
+    <t>Sitan kodi jwogi ibino reyo jo woko.</t>
+  </si>
+  <si>
+    <t>Joma winjo Were joleboth jobedi i piny pa Were manyien, kama lworo moro jye kobed’iye, piny ma lebed’iye genirok kodi mar.</t>
+  </si>
+  <si>
+    <t>Gikipiny mene ma Yesu chango owacho ma timere pama?</t>
+  </si>
+  <si>
+    <t>Ibino reyo woko jomarecho.</t>
+  </si>
+  <si>
+    <t>Joma Winjo Were Jobino Limo Silwany Mene i Hongo Mabino?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Par kwo gikipiny mabeyo minolimi i hongo ma bino ka iwinjo Jehova! </t>
+  </si>
+  <si>
+    <t>Jomarecho jokobedi, aka ibino geno kis dhano.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilebedo gi kwo maber; mongoye dhano moro jye ma two kosa mool. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Litho, rembo, kosa ywak jye kobedi. </t>
+  </si>
+  <si>
+    <t>Ongoye dhano moro jye ma leti to tho.</t>
+  </si>
+  <si>
+    <t>What Blessings Await Those Who Listen to God?</t>
+  </si>
+  <si>
+    <t>Imagine the future blessings that you will enjoy if you listen to Jehovah!</t>
+  </si>
+  <si>
+    <t>There will be no bad people, and you will be able to trust everyone.</t>
+  </si>
+  <si>
+    <t>There will be no pain, sorrow, or tears.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No one will grow old and die.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> You will be surrounded by friends and family. happy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will have perfect health; no one will be sick or infirm. </t>
+  </si>
+  <si>
+    <t>Life in Paradise will be a delight.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kwo i piny manyien bino kelo ri wan kisangala madit swa.</t>
+  </si>
+  <si>
+    <t>Ilebedo gi merin perin, wutimin in kanyachiel gi nyimerin.</t>
+  </si>
+  <si>
+    <t>Lworo moro jye kobed’iye.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ji jobino limo kisangala maradyeri.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There will be no fear. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">People will be truly </t>
+  </si>
+  <si>
+    <t>Jehova winjo kwayo mawan.</t>
+  </si>
+  <si>
+    <t>Go mito ni waluwi gi go munyo gima wawacho wok i chuny wan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jehova Winjo Kwayo Mawan? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ikiri ikway were moro jye kwanyo woko Jehova kende. </t>
+  </si>
+  <si>
+    <t>Yesu ofuonjo wan paka waripo kwayo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were winjo kwayo pa jomene? </t>
+  </si>
+  <si>
+    <t>Kwayi gima Were yenyo wotimere i piny paka timere i polo.</t>
+  </si>
+  <si>
+    <t>Inyalo kwayo go chiemo, tich, kabedo, ruk, kodikwo maber.</t>
+  </si>
+  <si>
+    <t>Kwayi Jehova wokonyin inyal timo gimaber.</t>
+  </si>
+  <si>
+    <t>Kwayi i nyingi Yesu inyuthi ni ifuoyo gima go otimo ri wan.</t>
+  </si>
+  <si>
+    <t>Jehova winjo kwayo pa joma timo gimotire</t>
+  </si>
+  <si>
+    <t>Ikiri irembi.</t>
+  </si>
+  <si>
+    <t>He wants us to speak to him from our hearts.</t>
+  </si>
+  <si>
+    <t>Jehovah listens to our prayers</t>
+  </si>
+  <si>
+    <t>Pray to Jehovah and not to anyone else.</t>
+  </si>
+  <si>
+    <t>Jesus taught us how to pray.​</t>
+  </si>
+  <si>
+    <t>To whom does God listen?​</t>
+  </si>
+  <si>
+    <t>Does Jehovah Listen to our prayers?</t>
+  </si>
+  <si>
+    <t>Pray that God’s will be done in heaven and on earth.</t>
+  </si>
+  <si>
+    <t>Pray in the name of Jesus to show that you value what he did for you</t>
+  </si>
+  <si>
+    <t>Ask Jehovah to help you do what is good.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> You can also pray about food, employment, shelter, clothing, and health.</t>
+  </si>
+  <si>
+    <t>Jehovah listens to people who do what is right.​</t>
+  </si>
+  <si>
+    <t>Do not be anxious.​</t>
+  </si>
+  <si>
+    <t>How Can You Have a Happy Family Life?</t>
+  </si>
+  <si>
+    <t>God’s standard is that marriage should be between one man and one woman.</t>
+  </si>
+  <si>
+    <t>A loving husband treats his wife with tenderness and understanding.</t>
+  </si>
+  <si>
+    <t>A wife should cooperate with her husband.</t>
+  </si>
+  <si>
+    <t>Children should obey their parents.</t>
+  </si>
+  <si>
+    <t>God’s Word says that a husband should love his wife as his own body and that a wife should have deep respect for her husband.</t>
+  </si>
+  <si>
+    <t>Sex outside the marriage arrangement is wrong.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Polygamy is also wrong.</t>
+  </si>
+  <si>
+    <t>Jehovah’s Word teaches families how to be happy.</t>
+  </si>
+  <si>
+    <t>Keep morally clean.​</t>
+  </si>
+  <si>
+    <t>Love, teach, and protect your children.​</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inyalo Limo Nedi Kisangala i Pecho Perin? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were mito ni nywomirok wobedi i dyer jachwo achiel gi dhako achiel. </t>
+  </si>
+  <si>
+    <t>Jachwo ma maro chiege woro chiege.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nyithindho joripo winjo jonywol pajo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dhako ripo tiyirok maber gi chwore.</t>
+  </si>
+  <si>
+    <t>Wikiri witimi chot.</t>
+  </si>
+  <si>
+    <t>Nywomo mon ma kalo achiel bende rach.</t>
+  </si>
+  <si>
+    <t>Mar nyithindho perin, ifuonji jo, kendo ikuri jo.</t>
+  </si>
+  <si>
+    <t>Wach pa Were fuonjo ji paka jonyalo limo kisangala i pechin pajo.</t>
+  </si>
+  <si>
+    <t>Dhano ka onindo gi ata kobedo dhako pere kosa chwore meno gimarach.</t>
+  </si>
+  <si>
+    <t>Wach pa Were wacho ni jachwo ripo maro chiege paka del kwoe won kendo ni dhako bende ripo miyo chwore dwo.</t>
+  </si>
+  <si>
+    <t>Ka Wamito ni Were Osangala Ginao ma Waripo Timo?</t>
+  </si>
+  <si>
+    <t>Ka wamaro Jehova wakiletimo gikipiny ma go kimiti.</t>
+  </si>
+  <si>
+    <t>Jehova kimiti ni wakwali, wameri, waor yen manyalo nyieko paro mawan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were dak nek, redho iyi jo, chwo nindo gi chwo wadi gin mon bende gi mon wadi gin. </t>
+  </si>
+  <si>
+    <t>Go kimiti wabedi jomawor kosa gorok  gi wadi wan.</t>
+  </si>
+  <si>
+    <t>Wakiripi lamo chal kosa thyedho.</t>
+  </si>
+  <si>
+    <t>Were paro nedi kwo thyeth?</t>
+  </si>
+  <si>
+    <t>Irao wakiripi lamo chal?</t>
+  </si>
+  <si>
+    <t>Joma timo gikipiny marecho jokobedi I piny pa Were manyien.</t>
+  </si>
+  <si>
+    <t>What Must We Do to Please God?</t>
+  </si>
+  <si>
+    <t>If we love Jehovah, we will not do things that he hates.</t>
+  </si>
+  <si>
+    <t>Jehovah does not want us to steal, to get drunk, or to abuse drugs.</t>
+  </si>
+  <si>
+    <t>We must not worship idols or practice spiritism.</t>
+  </si>
+  <si>
+    <t>In the earthly Paradise to come, there will be no place for people who do bad things.</t>
+  </si>
+  <si>
+    <t>He does not want us to be greedy or to fight with others.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">God hates murder, abortion, and homosexuality. </t>
+  </si>
+  <si>
+    <t>What is God’s view of magic?</t>
+  </si>
+  <si>
+    <t>Why should we not worship idols?</t>
+  </si>
+  <si>
+    <t>To be pleasing to God, we must try to be like him.</t>
+  </si>
+  <si>
+    <t>Show love to others by being kind and generous.</t>
+  </si>
+  <si>
+    <t>Be honest.</t>
+  </si>
+  <si>
+    <t>Be merciful and forgiving.</t>
+  </si>
+  <si>
+    <t>Tell others about Jehovah and his ways.​</t>
+  </si>
+  <si>
+    <t>Imitate Jehovah.</t>
+  </si>
+  <si>
+    <t>Show love.</t>
+  </si>
+  <si>
+    <t>Ka wamito ni Were osangala, waripo temo paka nyalere bedo paka go.</t>
+  </si>
+  <si>
+    <t>Bedi dhano ma ni gi mar kodi wor kendo japok.</t>
+  </si>
+  <si>
+    <t>Bedi dhano magenere.</t>
+  </si>
+  <si>
+    <t>Wach ri ji gima mako kwo Jehova kodi gima go mito niwatimi.</t>
+  </si>
+  <si>
+    <t>Bedi dhano ma mako wor ri ji kendo ma jachwak.</t>
+  </si>
+  <si>
+    <t>Bedi dhano male paka Jehova.</t>
+  </si>
+  <si>
+    <t>Nyuthi mar.</t>
+  </si>
+  <si>
+    <t>Inyalo Nyutho Nedi ni Iwinjo Jehova?</t>
+  </si>
+  <si>
+    <t>Kada nende kiyot timo ameno.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timi gima nyalere jye iweyi kula moro jye ma Baibul kiyeyere gine. </t>
+  </si>
+  <si>
+    <t>Ikiri idonji I wach maradhum ma piny rupiri joradhum jokithyel Jehova kodi Ker pere.</t>
+  </si>
+  <si>
+    <t>Jehova kuro joma winjo go.</t>
+  </si>
+  <si>
+    <t>Tiyere gi Wajulizi pa Jehova; jobino konyin chorok chiegin gi Were.</t>
+  </si>
+  <si>
+    <t>Medere fuonjirok gima mako kwo Were kendo itemi timo gima go yenyo.</t>
+  </si>
+  <si>
+    <t>Ka yeyo perin omedere, inyalo miyo Jehova kwo perin t’ilimo batisimo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soma Baibul,ikwayi Wajulizi pa Jehova jowokonyin nia gima Baibul fuonjo. </t>
+  </si>
+  <si>
+    <t>Ka inotimi ameno, ibino limo kwo makirum.</t>
+  </si>
+  <si>
+    <t>Kethi gikipiny mifuonjere i tim.</t>
+  </si>
+  <si>
+    <t>Wothi i royo matero jo I kwo</t>
+  </si>
+  <si>
+    <t>How Can You Show Loyalty to Jehovah?</t>
+  </si>
+  <si>
+    <t>It takes courage to do this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoid taking part in any customs that are not in agreement with the Bible. </t>
+  </si>
+  <si>
+    <t>Do not get involved in the political affairs of the nations; they do not support Jehovah and his Kingdom.</t>
+  </si>
+  <si>
+    <t>Associate with Jehovah’s Witnesses; they will help you draw close to God.</t>
+  </si>
+  <si>
+    <t>Continue to learn about God and try to obey his commandments.</t>
+  </si>
+  <si>
+    <t>Jehovah guards those loyal to him</t>
+  </si>
+  <si>
+    <t>When your faith has become strong, you should dedicate your life to Jehovah and get baptized.​</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read the Bible, and ask Jehovah’s Witnesses to help you understand it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then, apply what you learn. </t>
+  </si>
+  <si>
+    <t>If you do, you will live forever.</t>
+  </si>
+  <si>
+    <t>Ng'uti recho perin aka ey Were wochwak rin.</t>
+  </si>
+  <si>
+    <t>Repent and be forgiven.​</t>
+  </si>
+  <si>
+    <t>Walk on the road to life.</t>
+  </si>
+  <si>
+    <t>Ilimi Kwo Makirum</t>
+  </si>
+  <si>
+    <t>Live Forever</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -949,6 +2317,12 @@
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -980,7 +2354,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1001,6 +2375,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1298,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2504,4 +3884,1841 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E227"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
+      <selection activeCell="A211" sqref="A211"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="55.28515625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30">
+      <c r="A33" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30">
+      <c r="A34" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45">
+      <c r="A35" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30">
+      <c r="A36" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30">
+      <c r="A37" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="18">
+      <c r="A42" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="1:5" ht="30">
+      <c r="A43" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30">
+      <c r="A48" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30">
+      <c r="A49" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="30">
+      <c r="A58" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="30">
+      <c r="A61" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="30">
+      <c r="A66" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="30">
+      <c r="A67" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="30">
+      <c r="A68" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30">
+      <c r="A69" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="30">
+      <c r="A72" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="30">
+      <c r="A74" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="30">
+      <c r="A86" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>464</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="30">
+      <c r="A96" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>471</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="30">
+      <c r="A98" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="30">
+      <c r="A99" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="45">
+      <c r="A101" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>490</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="30">
+      <c r="A103" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="30">
+      <c r="A104" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="30">
+      <c r="A105" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="30">
+      <c r="A107" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="30">
+      <c r="A110" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="45">
+      <c r="A112" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="30">
+      <c r="A114" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="45">
+      <c r="A116" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="30">
+      <c r="A119" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="30">
+      <c r="A121" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="30">
+      <c r="A123" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="30">
+      <c r="A124" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>530</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="30">
+      <c r="A131" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="30">
+      <c r="A132" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="30">
+      <c r="A133" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="45">
+      <c r="A137" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="30">
+      <c r="A140" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="30">
+      <c r="A145" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="30">
+      <c r="A147" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="B148" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>575</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B153" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="30">
+      <c r="A155" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="30">
+      <c r="A156" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="30">
+      <c r="A157" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="30">
+      <c r="A159" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="45">
+      <c r="A162" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="30">
+      <c r="A165" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="30">
+      <c r="A166" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="30">
+      <c r="A167" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="30">
+      <c r="A168" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="30">
+      <c r="A177" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="B179" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>635</v>
+      </c>
+      <c r="B180" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="30">
+      <c r="A184" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="30">
+      <c r="A188" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="30">
+      <c r="A189" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>668</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="45">
+      <c r="A192" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="30">
+      <c r="A193" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="30">
+      <c r="A195" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="30">
+      <c r="A200" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="30">
+      <c r="A201" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="30">
+      <c r="A204" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="30">
+      <c r="A207" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="30">
+      <c r="A211" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="30">
+      <c r="A215" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="30">
+      <c r="A217" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="30">
+      <c r="A219" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="30">
+      <c r="A220" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="30">
+      <c r="A221" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="30">
+      <c r="A222" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>735</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added do you want to know the truth
</commit_message>
<xml_diff>
--- a/Jehovah Witness.xlsx
+++ b/Jehovah Witness.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="1" r:id="rId1"/>
     <sheet name="Common Verbs" sheetId="3" r:id="rId2"/>
     <sheet name="Listen to God" sheetId="4" r:id="rId3"/>
+    <sheet name="Know the truth" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="917">
   <si>
     <t>Adhola</t>
   </si>
@@ -2251,6 +2252,552 @@
   </si>
   <si>
     <t>Live Forever</t>
+  </si>
+  <si>
+    <t>Imito eyo Adyeri?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adyeri ma mako kwo ginao? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma mako kwo penji madongo ma ji jomaro penjere. </t>
+  </si>
+  <si>
+    <t>Miti ityeko penjereye penji me:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lweny kodi chandirok orumi?</t>
+  </si>
+  <si>
+    <t>Jomotho jo nikune?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odoko wanoneni ji mawan ma jotho? </t>
+  </si>
+  <si>
+    <t>Anyalo kwayo nedi aka Were Owinjan?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adyeri Were dewo kwo wan?   </t>
+  </si>
+  <si>
+    <t>Anyalo nedi limo kisangala i kwo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanyalo nwao kune radwok ma penji me? </t>
+  </si>
+  <si>
+    <t>Ka ipenjo ji mopokere opokere jodwoko penji no i nger mopokere.</t>
+  </si>
+  <si>
+    <t>Kada ipenji ji maryek kodi joma iworo, nger ma joledwokin
+kimakere.</t>
+  </si>
+  <si>
+    <t>Megi kwo radwok ma jomiyin nyalo neno p’otire to rumachien ma hongo machiek, inwao ni kotire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kareno, nitye kitawo achiel ma dwoko penji no maber swa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wach no a Baibul. </t>
+  </si>
+  <si>
+    <t>Medere kisoma ineni paka Baibul dwoko penji no i nger mayot kendo magenere.</t>
+  </si>
+  <si>
+    <t>Would You Like to Know the Truth?</t>
+  </si>
+  <si>
+    <t>THE truth about what?</t>
+  </si>
+  <si>
+    <t>Perhaps you have wondered about such questions as these:</t>
+  </si>
+  <si>
+    <t>About some of the most important questions that humans have ever asked.</t>
+  </si>
+  <si>
+    <t>Does God really care about us?</t>
+  </si>
+  <si>
+    <t>Will war and suffering ever end?</t>
+  </si>
+  <si>
+    <t>What happens to us when we die?</t>
+  </si>
+  <si>
+    <t>Is there any hope for the dead?</t>
+  </si>
+  <si>
+    <t>How can I pray and be heard by God?</t>
+  </si>
+  <si>
+    <t>How can I find happiness in life?</t>
+  </si>
+  <si>
+    <t>Where would you look for answers to these questions?</t>
+  </si>
+  <si>
+    <t>If you went to libraries or bookstores, you might find thousands of books claiming to provide the answers.</t>
+  </si>
+  <si>
+    <t>Often, though, one book contradicts another.</t>
+  </si>
+  <si>
+    <t>Others seem valid at the moment but soon become outdated and are revised or replaced.</t>
+  </si>
+  <si>
+    <t>There is, however, one book that contains reliable answers</t>
+  </si>
+  <si>
+    <t>It is a book of truth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus Christ said in prayer to God: “Your word is truth.”  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kitawo no obedo wach maradyeri. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo Yesu Kristo kwayo Were, owacho ni: “Wach perin obedo adyeri.” </t>
+  </si>
+  <si>
+    <t>On the following pages, you will get a glimpse of the Bible’s clear, truthful answers to the above questions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Today we know that Word as the Holy Bible. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adyeri Were Dewo Kwo Wan? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRAO JI JOPENJERE PENJI ME? </t>
+  </si>
+  <si>
+    <t>Din mathoth fuonjo ni Were ama kelo ri wan chandirok.</t>
+  </si>
+  <si>
+    <t>Does God Really Care About Us?</t>
+  </si>
+  <si>
+    <t>WHY THE QUESTION ARISES:</t>
+  </si>
+  <si>
+    <t>We live in a world full of cruelty and injustice. Many religions teach that the sufferings we experience are God’s will.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHAT THE BIBLE TEACHES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were kinyal timo gima kotire. </t>
+  </si>
+  <si>
+    <t>GIMA BAIBUL FUONJO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">God never causes what is wicked. </t>
+  </si>
+  <si>
+    <t>Nike Were kotire?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kameno be.</t>
+  </si>
+  <si>
+    <t>Were ni g’atoa maber ri ji.</t>
+  </si>
+  <si>
+    <t>Gima iyenyo wotimere i piny paka timere i polo.</t>
+  </si>
+  <si>
+    <t>Were dewo kwo wan tektek amomiyo otimo ri wan gikipiny mabeyo kweth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">God has a loving purpose for humans. </t>
+  </si>
+  <si>
+    <t>God cares so deeply about us that he has gone to great lengths to make the fulfillment of his purpose a certainty.</t>
+  </si>
+  <si>
+    <t>Let your will take place, as in heaven, also on earth.</t>
+  </si>
+  <si>
+    <t>That is why Jesus taught us to pray: “Our Father in the heavens, let . . . your kingdom come. "</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amomiyo Yesu ofuonjo wan kwayo ni: “Bawan mani polo, . . . Ker perin wobin."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is God unjust? </t>
+  </si>
+  <si>
+    <t>Not at all!</t>
+  </si>
+  <si>
+    <t>Romans 9:14 says: "What then shall we say? "</t>
+  </si>
+  <si>
+    <t>Joroma 9:14 wacho ni: “Onyo wawachi nedi?"</t>
+  </si>
+  <si>
+    <t>Lweny Kodi Chandirok Orumi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ji gana gi gana jomedere tho i lweny. </t>
+  </si>
+  <si>
+    <t>Wajojye wachandere.</t>
+  </si>
+  <si>
+    <t>Were chiko kelo syem i piny gipi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I Ker pa Were ma polo, ji jokilefuonjere lweny</t>
+  </si>
+  <si>
+    <t>Were bino chowo woko chandirok jye.</t>
+  </si>
+  <si>
+    <t>Will War and Suffering Ever End?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">War continues to claim untold numbers of human lives. </t>
+  </si>
+  <si>
+    <t>All of us have been touched by human suffering.</t>
+  </si>
+  <si>
+    <t>God foretells a time when he will establish peace earth wide</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Under his Kingdom, a heavenly government, people will not “learn war anymore.”</t>
+  </si>
+  <si>
+    <t>God will bring an end to all injustice and suffering.</t>
+  </si>
+  <si>
+    <t>Baibul wacho ni: Were bino yweyo pigi wa jo.</t>
+  </si>
+  <si>
+    <t>The former things including today’s injustices and sufferings have passed away.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tho odoko kobedi, kosa rembo, kosa litho, rupiri</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Bible promises: God will wipe out every tear from their eyes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death will be no more, neither will mourning nor outcry nor pain be anymore. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gikipiny machon kanyachiel gi chandirok ma wan’iye konon jotyeko leny woko.</t>
+  </si>
+  <si>
+    <t>What Happens to Us When We Die?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Some hold that the dead can harm the living or that God punishes the wicked by condemning them to eternal torment in a fiery hell.</t>
+  </si>
+  <si>
+    <t>Most of the world’s religions teach that something inside a person continues living after death.</t>
+  </si>
+  <si>
+    <t>At death, humans cease to exist.</t>
+  </si>
+  <si>
+    <t>Since the dead cannot know, feel, or experience anything, they cannot harm—or help—the living</t>
+  </si>
+  <si>
+    <t>Jomotho jo Nikune?</t>
+  </si>
+  <si>
+    <t>Din mathoth fuonjo ni ka dhano otho nitye gimoro i del pere aka ni gino kitho.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jomegi jofuonjo ni jomotho jonyalo chando jomakwo kosa ni Were wao jomarecho i mach makitho. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ka dhano otho, kwo pere rumo kichutho. </t>
+  </si>
+  <si>
+    <t>Jomotho jokinyal neno, winjo kosa timo gimoro jye, jochale pa dhano ma nindo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rupiri jomotho jokuya gimoro jye, jokinyal winjo kosa timo gimoro jye, jokinyal chando kosa konyo jomakwo., </t>
+  </si>
+  <si>
+    <t>The dead cannot see, hear or do anything, they are like people who are asleep</t>
+  </si>
+  <si>
+    <t>Odoko Wanoneni ji Mawan ma Jotho?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wamito kwo kendo wamito bedo kanyachiel gi merin mawan. </t>
+  </si>
+  <si>
+    <t>Kis ndir wamaro mito neno merin mawan ma chango jotho.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jomotho jobino chierino. </t>
+  </si>
+  <si>
+    <t>Yesu owacho ni: “Jomotho jye ma jonitye i kalyel jobino . . . wok kenyo.”</t>
+  </si>
+  <si>
+    <t>Paka obedo atoa pa Were, joma jolechierino jobino limo silwany ma bedo i piny pa Were manyien.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Baibul wacho ni: “Josilwany a joma mwol rupiri jobino lunjo piny.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chikirok me nyutho ni i hongo ma bino joma jolechierino jobino bedo gi kwo maber aka jobino bedo i piny chil gi chil.</t>
+  </si>
+  <si>
+    <t>Is There Any Hope for the Dead?</t>
+  </si>
+  <si>
+    <t>We want to live, and we want to enjoy life with those we love.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It is only natural that we yearn to see our dead loved ones again.</t>
+  </si>
+  <si>
+    <t>Those who have died will be resurrected.</t>
+  </si>
+  <si>
+    <t>In harmony with God’s original purpose, those resurrected as humans will have the opportunity to live on a paradise earth.</t>
+  </si>
+  <si>
+    <t>The Bible says: “The righteous will possess the earth, and they will live forever on it.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This promised future includes perfect health and everlasting life for obedient humans. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jesus promised that “those in the memorial tombs will . . . come out."</t>
+  </si>
+  <si>
+    <t>How Can I Pray and Be Heard by God?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People in practically all religions pray. </t>
+  </si>
+  <si>
+    <t>Yet, many feel that their prayers are not answered.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If we want God to listen to our prayers, we must pray in the way that he approves. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To do that, we need to learn what God’s will is and then pray accordingly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus taught us to avoid repeating set formulas in our prayers. </t>
+  </si>
+  <si>
+    <t>“When praying,” he said, “do not say the same things over and over again.”</t>
+  </si>
+  <si>
+    <t>Anyalo Kwayo Nedi aka Were Owinjan?</t>
+  </si>
+  <si>
+    <t>Chiegin ji i din jye jokwayo.</t>
+  </si>
+  <si>
+    <t>Kuchiel, joma thoth joparo ni Were kiwinji kwayo pajo.</t>
+  </si>
+  <si>
+    <t>Munyo Yesu fuonjo wan kwayo, owacho ni wakiripi oro “wach kweth” paka jomegi jotimo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meno nyutho ni wakiripi kiluda wach i kwayo mawan. </t>
+  </si>
+  <si>
+    <t>Ka wamito ni Were owinji kwayo mawan, waripo kwayo i nger ma go
+mito.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nyalo timo ameno, waripo fuonjere gima Were yenyo nyaka to wakwayo paka Were mito ni wakway go.</t>
+  </si>
+  <si>
+    <t>First John 5:14 explains: “No matter what we ask according to God’s will, he hears us.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 Yohana 5:14 wacho ni: “Waridho nike Were bino miyo wan gimoro jye ka wakwayo go paka go yenyo.”</t>
+  </si>
+  <si>
+    <t>Anyalo Nedi Limo Kisangala i Kwo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joma thoth joparo ni bedo gi ao, kosa eyirok, nyalo kelo ri jo kisangala. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ri ameno, jodwaro gikipiny no. </t>
+  </si>
+  <si>
+    <t>To rumachien jonwao ni gikipiny no kikeli kisangala.</t>
+  </si>
+  <si>
+    <t>Yesu onyutho gima kelo kisangala munyo wacho ni: “Josilwany meno a joma jowinjo Wach pa Were to joketho i tim.”</t>
+  </si>
+  <si>
+    <t>Ka wafuonjere Wach pa Were to waketho i tim walimo kisangala maradyeri kosa silwany</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ka waoro fuonji ma Baibul i kwo mawan, wanyalo limo kisangala.</t>
+  </si>
+  <si>
+    <t>Fuonjirok adyeri manitye i Baibul, konyo wan eyo gikipiny ma nyalo konyo wan i kwo.</t>
+  </si>
+  <si>
+    <t>How Can I Find Happiness in Life?</t>
+  </si>
+  <si>
+    <t>Many people believe that money, fame, or beauty will make them happy.</t>
+  </si>
+  <si>
+    <t>Jesus identified the key to happiness when he said: “Happy are those conscious of their spiritual need.” .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That truth is found in the Bible. </t>
+  </si>
+  <si>
+    <t>Knowing that truth can help us to discern what is really important and what is not.</t>
+  </si>
+  <si>
+    <t>So they pursue such things.</t>
+  </si>
+  <si>
+    <t>Later they find that those things don't bring happiness.</t>
+  </si>
+  <si>
+    <t>True happiness can be found If we study the word of God and act on it.</t>
+  </si>
+  <si>
+    <t>Adyeri no  nitye I Baibul</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Allowing Bible truth to guide our decisions and actions leads to a more meaningful life.</t>
+  </si>
+  <si>
+    <t>Watyeko nenoye paka Baibul dwoko penji auchiel no</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Imito ŋeyo maloyo kenyo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ka ibende ini gi riyo ma ŋeyo Wach pa Were, miti imaro penjere penji ma chalo ama</t>
+  </si>
+  <si>
+    <t>‘Bedi Were dewo kwoŋ wan, d’oweyo wachandere ama?</t>
+  </si>
+  <si>
+    <t>Baibul dwoko penji ma chalo ameno kodi penji megi i nger maber swa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anyalo nedi limo kisangala i pecho paran?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imito dhano wokonyin fuonjirok Baibul? </t>
+  </si>
+  <si>
+    <t>Wajulizi pa Jehova jonitye gi gikipiny aryo ma nyalo k</t>
+  </si>
+  <si>
+    <t>Marapena, obedo kitawo milwoŋo ni What Does the Bible Really Teach? mondiki konyo ji ŋeyo paka Baibul dwoko penji madongo ma wamaro penjere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mararyo, obedo chan ma fuonjo ji Baibul nono i pechin pajo. </t>
+  </si>
+  <si>
+    <t>Mujulizi pa Jehova ma bedo chiegin kodin nyalo wendo rin i pecho perin kosa kamoro jye to soma kodin Baibul.</t>
+  </si>
+  <si>
+    <t>Kisoma no bedo ma nono.</t>
+  </si>
+  <si>
+    <t>Kisoma me otyeko konyo ji gana gi gana i piny gipi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joma thoth jotundo kir wacho ni “Anwaŋo adyeri!” Ongoye ŋaŋo moro jye maloyo meno. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adyeri ma Baibul gonyo wan kwoŋ lworo moro jye ma wanyalo bedo gine. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miyo wan geno, kodi kisangala. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Yesu owacho ni: “Wibino ŋeyo adyeri aka adyeri no bino miyo wibedo i syem.”</t>
+  </si>
+  <si>
+    <t>This has been just a brief look at the Bible’s answers to six questions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Do you want to know more than that?</t>
+  </si>
+  <si>
+    <t>If you are among those “conscious of their spiritual need,” no doubt you do.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ‘If God cares about us, why has he allowed so much evil and suffering throughout history?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> How can I improve the quality of my family life?</t>
+  </si>
+  <si>
+    <t>The Bible gives full and satisfying answers to these and many more questions.</t>
+  </si>
+  <si>
+    <t>However, many today hesitate to look into the Bible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kareno, joma thoth jokimiti kisoma Baibul. </t>
+  </si>
+  <si>
+    <t>Joparo ni Baibul obedo kitawo madwoŋ swa kendo matek.</t>
+  </si>
+  <si>
+    <t>They see it as a lengthy book that is sometimes hard to understand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Would you like help to find the answers in the Bible? </t>
+  </si>
+  <si>
+    <t>Jehovah’s Witnesses offer two tools that can assist you.</t>
+  </si>
+  <si>
+    <t>First, the book What Does the Bible Really Teach? is designed to help busy people to examine the Bible’s clear answers to vital questions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The second tool is a free program of home Bible study. </t>
+  </si>
+  <si>
+    <t>The study is free of charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A jehovah witness next to youcan come to your home or another convenient location and  discuss the Bible with you. </t>
+  </si>
+  <si>
+    <t>Millions of people the world over have benefited from this program</t>
+  </si>
+  <si>
+    <t>Many of them have come to this thrilling conclusion: “I have found the truth!”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bible truth liberates us from superstition, confusion, and morbid fear. </t>
+  </si>
+  <si>
+    <t>It gives us hope, purpose, and joy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jesus said: “You will know the truth, and the truth will set you free.”</t>
   </si>
 </sst>
 </file>
@@ -3891,7 +4438,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
+    <sheetView topLeftCell="A210" workbookViewId="0">
       <selection activeCell="A211" sqref="A211"/>
     </sheetView>
   </sheetViews>
@@ -3932,7 +4479,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="30">
       <c r="A5" s="2" t="s">
         <v>337</v>
       </c>
@@ -3980,7 +4527,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="30">
       <c r="A11" s="2" t="s">
         <v>294</v>
       </c>
@@ -4004,7 +4551,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="30">
       <c r="A14" s="2" t="s">
         <v>299</v>
       </c>
@@ -4012,7 +4559,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="30">
       <c r="A15" s="2" t="s">
         <v>302</v>
       </c>
@@ -4044,7 +4591,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="30">
       <c r="A19" s="2" t="s">
         <v>309</v>
       </c>
@@ -4052,7 +4599,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="30">
       <c r="A20" s="2" t="s">
         <v>310</v>
       </c>
@@ -4108,7 +4655,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" ht="30">
       <c r="A27" s="2" t="s">
         <v>325</v>
       </c>
@@ -4164,7 +4711,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30">
+    <row r="34" spans="1:5" ht="45">
       <c r="A34" s="2" t="s">
         <v>354</v>
       </c>
@@ -4212,7 +4759,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" ht="30">
       <c r="A40" s="2" t="s">
         <v>361</v>
       </c>
@@ -4220,7 +4767,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="2" t="s">
         <v>363</v>
       </c>
@@ -4365,7 +4912,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" ht="30">
       <c r="A59" s="2" t="s">
         <v>400</v>
       </c>
@@ -4389,7 +4936,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" ht="30">
       <c r="A62" s="2" t="s">
         <v>407</v>
       </c>
@@ -4437,7 +4984,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="30">
+    <row r="68" spans="1:2" ht="45">
       <c r="A68" s="2" t="s">
         <v>413</v>
       </c>
@@ -4469,7 +5016,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="30">
+    <row r="72" spans="1:2" ht="45">
       <c r="A72" s="13" t="s">
         <v>425</v>
       </c>
@@ -4485,7 +5032,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="30">
+    <row r="74" spans="1:2" ht="45">
       <c r="A74" s="2" t="s">
         <v>428</v>
       </c>
@@ -5357,7 +5904,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" ht="30">
       <c r="A183" s="2" t="s">
         <v>637</v>
       </c>
@@ -5715,6 +6262,751 @@
       </c>
       <c r="B227" s="2" t="s">
         <v>735</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:B93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="67" style="2" customWidth="1"/>
+    <col min="2" max="2" width="58" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30">
+      <c r="A4" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30">
+      <c r="A13" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30">
+      <c r="A14" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30">
+      <c r="A20" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30">
+      <c r="A23" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30">
+      <c r="A30" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="30">
+      <c r="A32" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30">
+      <c r="A37" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="30">
+      <c r="A39" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="30">
+      <c r="A40" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="30">
+      <c r="A41" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="30">
+      <c r="A43" t="s">
+        <v>822</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="45">
+      <c r="A44" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30">
+      <c r="A46" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30">
+      <c r="A47" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="30">
+      <c r="A50" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="30">
+      <c r="A52" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="30">
+      <c r="A53" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="30">
+      <c r="A54" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="30">
+      <c r="A55" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="30">
+      <c r="A59" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="30">
+      <c r="A60" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="30">
+      <c r="A61" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="30">
+      <c r="A62" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30">
+      <c r="A63" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="30">
+      <c r="A65" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="30">
+      <c r="A68" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30">
+      <c r="A69" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="30">
+      <c r="A71" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="30">
+      <c r="A72" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30">
+      <c r="A73" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="30">
+      <c r="A75" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="30">
+      <c r="A76" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="30">
+      <c r="A78" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="30">
+      <c r="A80" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="30">
+      <c r="A81" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="45">
+      <c r="A83" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="30">
+      <c r="A85" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="30">
+      <c r="A87" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="30">
+      <c r="A88" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="30">
+      <c r="A89" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="30">
+      <c r="A91" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="2" t="s">
+        <v>894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created legal texts and added offer letter
</commit_message>
<xml_diff>
--- a/Jehovah Witness.xlsx
+++ b/Jehovah Witness.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="925">
   <si>
     <t>Adhola</t>
   </si>
@@ -802,13 +802,7 @@
     <t>To rupiri were am’ociko wan kwo makirum, wakiripi yeyo dhano moro je cero wan fongirok gima mako kwoŋ kwo no​</t>
   </si>
   <si>
-    <t>Read Proverbs 29:25; Revelation 14:6, 7</t>
-  </si>
-  <si>
     <t>But the opportunity of a better future is too good to miss</t>
-  </si>
-  <si>
-    <t>Soma Agecin 29:25; Menyirok 14:6, 7</t>
   </si>
   <si>
     <t>Soma 2 Timothe 3:1-5</t>
@@ -2798,6 +2792,36 @@
   </si>
   <si>
     <t xml:space="preserve"> Jesus said: “You will know the truth, and the truth will set you free.”</t>
+  </si>
+  <si>
+    <t>God wants you to be His friend.</t>
+  </si>
+  <si>
+    <t>He will help you get happiness in life.</t>
+  </si>
+  <si>
+    <t>God can help you know what you want and you don't want.</t>
+  </si>
+  <si>
+    <t>The new world will not be like the one we are in today</t>
+  </si>
+  <si>
+    <t>What shows?</t>
+  </si>
+  <si>
+    <t>What the Bible tells us about the floods during Noah's time teaches us what?</t>
+  </si>
+  <si>
+    <t>How does the new world looks like?</t>
+  </si>
+  <si>
+    <t>He will help you know what you did in the past, what you are doing now and what you will do in the future</t>
+  </si>
+  <si>
+    <t>Soma Agecin gi Menyirok 14:6, 7</t>
+  </si>
+  <si>
+    <t>Read Proverbs and Revelation 14:6</t>
   </si>
 </sst>
 </file>
@@ -3223,10 +3247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B104"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3905,7 +3929,7 @@
         <v>238</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -3926,18 +3950,18 @@
     </row>
     <row r="87" spans="1:2" ht="30">
       <c r="A87" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -3985,55 +4009,79 @@
         <v>255</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2" t="s">
-        <v>258</v>
+        <v>923</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="30">
+      <c r="A98" s="10" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="2" t="s">
+      <c r="B98" s="2" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="30">
+      <c r="A99" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" ht="15.75">
-      <c r="A99" s="10" t="s">
+      <c r="B99" s="2" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="30">
+      <c r="A100" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" ht="30">
-      <c r="A100" s="2" t="s">
+      <c r="B101" s="2" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="30">
+      <c r="A102" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" ht="30">
-      <c r="A103" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" s="3" t="s">
-        <v>283</v>
+      <c r="B102" s="2" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -4046,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4375,50 +4423,50 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B41" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B42" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B43" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30">
       <c r="A44" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B45" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -4439,7 +4487,7 @@
   <dimension ref="A1:E227"/>
   <sheetViews>
     <sheetView topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="A211" sqref="A211"/>
+      <selection activeCell="E220" sqref="E220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4457,1811 +4505,1811 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
       <c r="A5" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
       <c r="A11" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30">
       <c r="A14" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
       <c r="A15" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30">
       <c r="A19" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
       <c r="A20" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
       <c r="A27" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30">
       <c r="A33" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="45">
       <c r="A34" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="45">
       <c r="A35" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30">
       <c r="A36" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30">
       <c r="A37" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30">
       <c r="A39" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30">
       <c r="A40" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30">
       <c r="A41" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18">
       <c r="A42" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E42" s="12"/>
     </row>
     <row r="43" spans="1:5" ht="30">
       <c r="A43" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30">
       <c r="A44" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30">
       <c r="A48" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="30">
       <c r="A49" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30">
       <c r="A58" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="30">
       <c r="A59" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30">
       <c r="A61" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="30">
       <c r="A62" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="30">
       <c r="A66" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="30">
       <c r="A67" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="45">
       <c r="A68" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30">
       <c r="A69" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="45">
       <c r="A72" s="13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="45">
       <c r="A74" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="30">
       <c r="A86" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>460</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="30">
       <c r="A96" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="30">
       <c r="A98" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="30">
       <c r="A99" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="45">
       <c r="A101" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="30">
       <c r="A103" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="30">
       <c r="A104" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="30">
       <c r="A105" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="30">
       <c r="A107" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="30">
       <c r="A110" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="45">
       <c r="A112" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="30">
       <c r="A114" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="45">
       <c r="A116" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="30">
       <c r="A119" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="30">
       <c r="A121" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="30">
       <c r="A123" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="30">
       <c r="A124" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="30">
       <c r="A131" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="30">
       <c r="A132" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="30">
       <c r="A133" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="45">
       <c r="A137" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="30">
       <c r="A140" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="30">
       <c r="A145" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="30">
       <c r="A147" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B148" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B153" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="30">
       <c r="A155" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="30">
       <c r="A156" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="30">
       <c r="A157" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="30">
       <c r="A159" s="2" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="45">
       <c r="A162" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="30">
       <c r="A165" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="30">
       <c r="A166" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="30">
       <c r="A167" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="30">
       <c r="A168" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>626</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>627</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="30">
       <c r="A177" s="2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="2" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="2" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B179" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B180" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="30">
       <c r="A183" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="30">
       <c r="A184" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="2" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="30">
       <c r="A188" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="30">
       <c r="A189" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="45">
       <c r="A192" s="2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="30">
       <c r="A193" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="30">
       <c r="A195" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="2" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="2" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="30">
       <c r="A200" s="2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="30">
       <c r="A201" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="30">
       <c r="A204" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="2" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="2" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="30">
       <c r="A207" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="30">
       <c r="A211" s="2" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="2" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="2" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="30">
       <c r="A215" s="2" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="30">
       <c r="A217" s="2" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="30">
       <c r="A219" s="2" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="30">
       <c r="A220" s="2" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="30">
       <c r="A221" s="2" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="30">
       <c r="A222" s="2" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="2" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="2" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="2" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="2" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
   </sheetData>
@@ -6286,727 +6334,727 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30">
       <c r="A4" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
       <c r="A13" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30">
       <c r="A14" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
       <c r="A15" s="2" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
       <c r="A20" s="2" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30">
       <c r="A23" s="2" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>781</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30">
       <c r="A30" s="2" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
       <c r="A32" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>788</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30">
       <c r="A37" s="2" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="30">
       <c r="A39" s="2" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30">
       <c r="A40" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>812</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="30">
       <c r="A41" s="2" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="30">
       <c r="A43" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="45">
       <c r="A44" s="2" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30">
       <c r="A46" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>825</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30">
       <c r="A47" s="2" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
       <c r="A50" s="2" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="30">
       <c r="A52" s="2" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="30">
       <c r="A53" s="2" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30">
       <c r="A54" s="2" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30">
       <c r="A55" s="2" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="30">
       <c r="A59" s="2" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30">
       <c r="A60" s="2" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30">
       <c r="A61" s="2" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="30">
       <c r="A62" s="2" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="30">
       <c r="A63" s="2" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="30">
       <c r="A65" s="2" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="30">
       <c r="A68" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30">
       <c r="A69" s="2" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="30">
       <c r="A71" s="2" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30">
       <c r="A72" s="2" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="30">
       <c r="A73" s="2" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="30">
       <c r="A75" s="2" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="30">
       <c r="A76" s="2" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="30">
       <c r="A78" s="2" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="30">
       <c r="A80" s="2" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="30">
       <c r="A81" s="2" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="45">
       <c r="A83" s="2" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="30">
       <c r="A85" s="2" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="30">
       <c r="A87" s="2" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="30">
       <c r="A88" s="2" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="30">
       <c r="A89" s="2" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="30">
       <c r="A91" s="2" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>